<commit_message>
Fixed sampling of sediment grids
</commit_message>
<xml_diff>
--- a/project/test/cases_test.xlsx
+++ b/project/test/cases_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/project/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCEE723-4D0C-F347-A891-CC5862212CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5EFEFC-043D-B040-BFDE-15290E250721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{0A9D0FCF-1F4B-5247-B35D-CBB46409C9D9}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{0A9D0FCF-1F4B-5247-B35D-CBB46409C9D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Sediment subduction</t>
+  </si>
+  <si>
+    <t>sed</t>
+  </si>
+  <si>
+    <t>Sample sediment grid</t>
+  </si>
+  <si>
+    <t>syn</t>
+  </si>
+  <si>
+    <t>Reconstructed motions</t>
+  </si>
+  <si>
+    <t>sediment thickness</t>
   </si>
 </sst>
 </file>
@@ -413,22 +431,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D861B8B-A8AA-1B4E-A7D6-DBD232E13F33}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed calculation of plate velocity
Still stuck on calculating synthetic stage rotation, error must be somewhere in the summing of the torques (because the sum is the same for all plates, regardless of the x, y, z components.
</commit_message>
<xml_diff>
--- a/project/test/cases_test.xlsx
+++ b/project/test/cases_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/project/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5EFEFC-043D-B040-BFDE-15290E250721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA74A06-490D-8F43-B488-D80D224224DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{0A9D0FCF-1F4B-5247-B35D-CBB46409C9D9}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>